<commit_message>
Commiting all the test cases, data
</commit_message>
<xml_diff>
--- a/PatternObjectModel/data/TC001.xlsx
+++ b/PatternObjectModel/data/TC001.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="15300" windowHeight="4050"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -41,36 +41,12 @@
   <si>
     <t>Demo Sales Manager</t>
   </si>
-  <si>
-    <t>companyName</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>expectedText</t>
-  </si>
-  <si>
-    <t>testcompany</t>
-  </si>
-  <si>
-    <t>testFN</t>
-  </si>
-  <si>
-    <t>testLN</t>
-  </si>
-  <si>
-    <t>testcompany1</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,7 +69,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,40 +92,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -196,7 +152,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,10 +184,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,7 +218,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,25 +393,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,20 +416,8 @@
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -490,20 +427,8 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -512,18 +437,6 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -533,24 +446,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>